<commit_message>
Did some more playtesting yesterday.
</commit_message>
<xml_diff>
--- a/Custom Cards/Horus the Black Flame Dragon/Playtest Results - Horus Control.xlsx
+++ b/Custom Cards/Horus the Black Flame Dragon/Playtest Results - Horus Control.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Custom Cards\Horus the Black Flame Dragon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6EB63D-EB12-4F86-8686-3EB21022BD14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C040BD-1027-4C77-A817-BC8055E0AF53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23040" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="3" xr2:uid="{AD9CF55C-5A2C-43F9-8449-28DA4DBE7F5E}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{AD9CF55C-5A2C-43F9-8449-28DA4DBE7F5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Environment Changes" sheetId="6" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="91">
   <si>
     <t>Deck</t>
   </si>
@@ -882,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC8C623-D4B8-4C22-A988-D9BD9517564D}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,8 +1790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E830D7-F746-4F8D-8170-0D055311D58C}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1959,34 +1959,261 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
+      <c r="A7" s="9">
+        <v>45626</v>
+      </c>
+      <c r="B7" s="4">
+        <v>38565</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
+      <c r="A8" s="9">
+        <v>45626</v>
+      </c>
+      <c r="B8" s="4">
+        <v>38565</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
+      <c r="A9" s="9">
+        <v>45626</v>
+      </c>
+      <c r="B9" s="4">
+        <v>38565</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="4"/>
+      <c r="A10" s="9">
+        <v>45626</v>
+      </c>
+      <c r="B10" s="4">
+        <v>38565</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
+      <c r="A11" s="9">
+        <v>45626</v>
+      </c>
+      <c r="B11" s="4">
+        <v>38565</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
+      <c r="A12" s="9">
+        <v>45626</v>
+      </c>
+      <c r="B12" s="4">
+        <v>38565</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
+      <c r="A13" s="9">
+        <v>45626</v>
+      </c>
+      <c r="B13" s="4">
+        <v>38565</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
+      <c r="A14" s="9">
+        <v>45626</v>
+      </c>
+      <c r="B14" s="4">
+        <v>38565</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
+      <c r="A15" s="9">
+        <v>45626</v>
+      </c>
+      <c r="B15" s="4">
+        <v>38565</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
+      <c r="A16" s="9">
+        <v>45626</v>
+      </c>
+      <c r="B16" s="4">
+        <v>38565</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H16">

</xml_diff>